<commit_message>
LC AMJ'22 QBR update
</commit_message>
<xml_diff>
--- a/Excel Files/LL QBR AMJ.xlsx
+++ b/Excel Files/LL QBR AMJ.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Capillary\Linen Club\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Linen-Club\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="3564" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="business overview" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,15 @@
     <sheet name="Category wise Sales" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Category wise Sales'!$A$30:$D$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Category wise Sales'!$A$35:$D$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Second Visit Study'!$A$1:$C$20</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
   <si>
     <t>customers_shopped</t>
   </si>
@@ -119,109 +119,10 @@
     <t>UNCLASSIFIED</t>
   </si>
   <si>
-    <t>SHIRT</t>
-  </si>
-  <si>
-    <t>Trousers</t>
-  </si>
-  <si>
-    <t>Khakis</t>
-  </si>
-  <si>
-    <t>Innerwear - Trunk</t>
-  </si>
-  <si>
-    <t>Tie</t>
-  </si>
-  <si>
-    <t>Suits</t>
-  </si>
-  <si>
-    <t>Jackets</t>
-  </si>
-  <si>
-    <t>Footwear - Sandals</t>
-  </si>
-  <si>
-    <t>Footwear   Derby</t>
-  </si>
-  <si>
-    <t>BOTTOM</t>
-  </si>
-  <si>
-    <t>Footwear   Oxford</t>
-  </si>
-  <si>
-    <t>Sweat-Shirt</t>
-  </si>
-  <si>
-    <t>Jeans</t>
-  </si>
-  <si>
-    <t>T Shirt</t>
-  </si>
-  <si>
-    <t>Belt</t>
-  </si>
-  <si>
-    <t>Socks</t>
-  </si>
-  <si>
-    <t>Footwear   Slip On</t>
-  </si>
-  <si>
-    <t>Waist Coat</t>
-  </si>
-  <si>
-    <t>Pocket Square</t>
-  </si>
-  <si>
-    <t>MASK</t>
-  </si>
-  <si>
-    <t>FORMAL</t>
-  </si>
-  <si>
-    <t>AFI</t>
-  </si>
-  <si>
-    <t>CASUALE</t>
-  </si>
-  <si>
-    <t>FORMAL-NOS</t>
-  </si>
-  <si>
-    <t>URBAN</t>
-  </si>
-  <si>
-    <t>CASUALE-NOS</t>
-  </si>
-  <si>
-    <t>FORMAL-LUXE</t>
-  </si>
-  <si>
     <t>INVALID</t>
   </si>
   <si>
     <t>% Sales</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>Loafers</t>
-  </si>
-  <si>
-    <t>Sneakers</t>
-  </si>
-  <si>
-    <t>Sweater</t>
-  </si>
-  <si>
-    <t>Zipper Jacket</t>
   </si>
   <si>
     <t>MOM Top Loyalists Shopped</t>
@@ -283,11 +184,41 @@
   <si>
     <t>Stitch</t>
   </si>
+  <si>
+    <t>Saree</t>
+  </si>
+  <si>
+    <t>Chambray</t>
+  </si>
+  <si>
+    <t>Stripe</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Solid/Chambray</t>
+  </si>
+  <si>
+    <t>Full Sleve</t>
+  </si>
+  <si>
+    <t>Digital Print</t>
+  </si>
+  <si>
+    <t>Half Sleve</t>
+  </si>
+  <si>
+    <t>cat_design</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
@@ -899,7 +830,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1026,7 +957,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -1082,7 +1013,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E2FC-448E-A4F6-AC1EF66EEC06}"/>
             </c:ext>
@@ -1145,7 +1076,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -1201,7 +1132,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E2FC-448E-A4F6-AC1EF66EEC06}"/>
             </c:ext>
@@ -1218,11 +1149,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1245275039"/>
-        <c:axId val="1245275871"/>
+        <c:axId val="595404432"/>
+        <c:axId val="595408240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1245275039"/>
+        <c:axId val="595404432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1245275871"/>
+        <c:crossAx val="595408240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1270,7 +1201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1245275871"/>
+        <c:axId val="595408240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1318,7 +1249,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1245275039"/>
+        <c:crossAx val="595404432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1401,7 +1332,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1539,7 +1470,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -1590,18 +1521,18 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7085</c:v>
+                  <c:v>7004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7310</c:v>
+                  <c:v>7288</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12352</c:v>
+                  <c:v>12455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6C35-4386-AEE7-34814E6ABE3F}"/>
             </c:ext>
@@ -1669,7 +1600,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -1720,18 +1651,18 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2044</c:v>
+                  <c:v>2031</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2267</c:v>
+                  <c:v>2258</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5288</c:v>
+                  <c:v>5310</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6C35-4386-AEE7-34814E6ABE3F}"/>
             </c:ext>
@@ -1748,11 +1679,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1154915215"/>
-        <c:axId val="1154916879"/>
+        <c:axId val="595405520"/>
+        <c:axId val="595404976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1154915215"/>
+        <c:axId val="595405520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1795,7 +1726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1154916879"/>
+        <c:crossAx val="595404976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1803,7 +1734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1154916879"/>
+        <c:axId val="595404976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1854,7 +1785,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1154915215"/>
+        <c:crossAx val="595405520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1936,7 +1867,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2079,7 +2010,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -2135,7 +2066,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FDD9-4364-B97F-807CF17B3FA5}"/>
             </c:ext>
@@ -2203,7 +2134,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -2259,7 +2190,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FDD9-4364-B97F-807CF17B3FA5}"/>
             </c:ext>
@@ -2276,11 +2207,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1238743615"/>
-        <c:axId val="1238740703"/>
+        <c:axId val="595415312"/>
+        <c:axId val="595408784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1238743615"/>
+        <c:axId val="595415312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2323,7 +2254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238740703"/>
+        <c:crossAx val="595408784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2331,7 +2262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1238740703"/>
+        <c:axId val="595408784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2382,7 +2313,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238743615"/>
+        <c:crossAx val="595415312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5000"/>
@@ -2465,7 +2396,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2603,7 +2534,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -2659,7 +2590,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-27C1-424E-AE6F-BE297C0D192C}"/>
             </c:ext>
@@ -2727,7 +2658,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -2783,7 +2714,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-27C1-424E-AE6F-BE297C0D192C}"/>
             </c:ext>
@@ -2800,11 +2731,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1248345151"/>
-        <c:axId val="1248347231"/>
+        <c:axId val="595410416"/>
+        <c:axId val="595412048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1248345151"/>
+        <c:axId val="595410416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2847,7 +2778,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1248347231"/>
+        <c:crossAx val="595412048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2855,7 +2786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1248347231"/>
+        <c:axId val="595412048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2906,7 +2837,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1248345151"/>
+        <c:crossAx val="595410416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2988,7 +2919,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3126,7 +3057,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -3182,7 +3113,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8897-45D1-9CC8-ACFB43C8E48F}"/>
             </c:ext>
@@ -3250,7 +3181,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -3306,7 +3237,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8897-45D1-9CC8-ACFB43C8E48F}"/>
             </c:ext>
@@ -3323,11 +3254,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1458782911"/>
-        <c:axId val="1458777087"/>
+        <c:axId val="595415856"/>
+        <c:axId val="472087056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1458782911"/>
+        <c:axId val="595415856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3370,7 +3301,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1458777087"/>
+        <c:crossAx val="472087056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3378,7 +3309,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1458777087"/>
+        <c:axId val="472087056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3429,7 +3360,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1458782911"/>
+        <c:crossAx val="595415856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3511,7 +3442,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3525,6 +3456,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Top Ten Purchased By People In their Second Visit</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3652,7 +3613,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2F17-460C-BEEE-3DB5B6F9083B}"/>
             </c:ext>
@@ -3668,11 +3629,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2134629311"/>
-        <c:axId val="2134630975"/>
+        <c:axId val="649537072"/>
+        <c:axId val="649538704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134629311"/>
+        <c:axId val="649537072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3715,7 +3676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134630975"/>
+        <c:crossAx val="649538704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3723,7 +3684,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134630975"/>
+        <c:axId val="649538704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3774,7 +3735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134629311"/>
+        <c:crossAx val="649537072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3824,450 +3785,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1"/>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-FCC7-421D-BEAF-16EC08DEA001}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-8D5B-4C1C-B8A3-943DE15CEAB6}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-8D5B-4C1C-B8A3-943DE15CEAB6}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-8D5B-4C1C-B8A3-943DE15CEAB6}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-8D5B-4C1C-B8A3-943DE15CEAB6}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-8D5B-4C1C-B8A3-943DE15CEAB6}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="60000"/>
-                      <a:lumOff val="40000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-FCC7-421D-BEAF-16EC08DEA001}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="bestFit"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Category wise Sales'!$A$3:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="1">
-                  <c:v>FORMAL</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>FORMAL-NOS</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>AFI</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>CASUALE</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>URBAN</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>CASUALE-NOS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Category wise Sales'!$D$3:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="1">
-                  <c:v>0.45994905902403643</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.24995809163005861</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.14035992277742862</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.10604871325117979</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6029801361474696E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6807563550451401E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8D5B-4C1C-B8A3-943DE15CEAB6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="bestFit"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:pattFill prst="dkDnDiag">
-      <a:fgClr>
-        <a:schemeClr val="lt1"/>
-      </a:fgClr>
-      <a:bgClr>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="10000"/>
-          <a:lumOff val="90000"/>
-        </a:schemeClr>
-      </a:bgClr>
-    </a:pattFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4286,13 +3804,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -4300,14 +3832,44 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-IN" sz="1200" b="0" i="0" baseline="0">
+              <a:rPr lang="en-IN" sz="1100" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Top 5 Formal Categories and % Contribution </a:t>
+              <a:t>Shirting Categories &amp; % Contribution </a:t>
             </a:r>
-            <a:endParaRPr lang="en-IN" sz="1200">
+            <a:endParaRPr lang="en-IN" sz="1100">
               <a:effectLst/>
             </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IN" sz="1100"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4324,13 +3886,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -4363,11 +3939,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-AA3D-42C3-86C5-AAE25500BCC2}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4383,11 +3954,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-AA3D-42C3-86C5-AAE25500BCC2}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4403,11 +3969,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-AA3D-42C3-86C5-AAE25500BCC2}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -4423,11 +3984,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-AA3D-42C3-86C5-AAE25500BCC2}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -4443,11 +3999,21 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-AA3D-42C3-86C5-AAE25500BCC2}"/>
-              </c:ext>
-            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -4509,56 +4075,57 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Category wise Sales'!$B$18:$B$22</c:f>
+              <c:f>'Category wise Sales'!$B$27:$B$32</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Jackets</c:v>
+                  <c:v>Chambray</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SHIRT</c:v>
+                  <c:v>Stripe</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Trousers</c:v>
+                  <c:v>Solid</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Suits</c:v>
+                  <c:v>Check</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Waist Coat</c:v>
+                  <c:v>Solid/Chambray</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Others</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Category wise Sales'!$E$18:$E$22</c:f>
+              <c:f>'Category wise Sales'!$E$27:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.4650900892377488</c:v>
+                  <c:v>0.31768745851857477</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31831235755560222</c:v>
+                  <c:v>0.23631984393633496</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1951455267075031</c:v>
+                  <c:v>0.19395878362250094</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.71257636755449E-2</c:v>
+                  <c:v>0.12235504497039888</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3262628236008542E-3</c:v>
+                  <c:v>7.2904200457121843E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6774668495068598E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5EB8-4285-9CAC-DEA68761CF75}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="bestFit"/>
@@ -4649,8 +4216,8 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4670,7 +4237,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4683,12 +4250,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-IN" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-IN" sz="1100" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Top 5 Casuale Categories &amp; % Contribution </a:t>
+              <a:t>Suiting Categories &amp; % Contribution </a:t>
             </a:r>
-            <a:endParaRPr lang="en-IN">
+            <a:endParaRPr lang="en-IN" sz="1100">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -4708,7 +4275,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4746,11 +4313,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-EFC0-4FF8-839C-7AF25071136D}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4766,11 +4328,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-EFC0-4FF8-839C-7AF25071136D}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4786,51 +4343,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-EFC0-4FF8-839C-7AF25071136D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-EFC0-4FF8-839C-7AF25071136D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-EFC0-4FF8-839C-7AF25071136D}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -4892,56 +4404,39 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Category wise Sales'!$B$35:$B$52</c:f>
+              <c:f>'Category wise Sales'!$B$36:$B$38</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Khakis</c:v>
+                  <c:v>Chambray</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SHIRT</c:v>
+                  <c:v>Solid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Sweat-Shirt</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Jackets</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>T Shirt</c:v>
+                  <c:v>Check</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Category wise Sales'!$E$35:$E$52</c:f>
+              <c:f>'Category wise Sales'!$E$36:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.20123209274142945</c:v>
+                  <c:v>0.56861718734885203</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8916205034877739E-2</c:v>
+                  <c:v>0.27919588530889522</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8051408914736529E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0673426845943975E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.3611044859299805E-3</c:v>
+                  <c:v>0.15218692734225273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E113-4BCB-AC9E-C55FC3D402C8}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="bestFit"/>
@@ -5340,46 +4835,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -8399,549 +7854,6 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="256">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="dkDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="lt1"/>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="10000"/>
-            <a:lumOff val="90000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr"/>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr"/>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-      <a:ln w="50800">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="15875">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="800" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:alpha val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="0" normalizeH="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9460,7 +8372,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10179,19 +9091,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>39756</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>69574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>496955</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10209,19 +9121,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>437322</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>145775</xdr:rowOff>
+      <xdr:colOff>19878</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9939</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>198783</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142461</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>470452</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>46383</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10231,36 +9143,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>298175</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>178903</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>72887</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>33130</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10535,7 +9417,7 @@
   <dimension ref="A2:D30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10755,7 +9637,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="1">
-        <v>56616</v>
+        <v>56615</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="19.2" x14ac:dyDescent="0.3">
@@ -10769,7 +9651,7 @@
         <v>8</v>
       </c>
       <c r="D25" s="1">
-        <v>26837</v>
+        <v>7850</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="19.2" x14ac:dyDescent="0.3">
@@ -10806,8 +9688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10818,7 +9700,7 @@
   <sheetData>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B6" s="22"/>
     </row>
@@ -10878,7 +9760,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1">
         <v>90</v>
@@ -10892,10 +9774,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>7085</v>
+        <v>7004</v>
       </c>
       <c r="C23" s="1">
-        <v>2044</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -10903,10 +9785,10 @@
         <v>15</v>
       </c>
       <c r="B24" s="1">
-        <v>7310</v>
+        <v>7288</v>
       </c>
       <c r="C24" s="1">
-        <v>2267</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -10914,10 +9796,10 @@
         <v>14</v>
       </c>
       <c r="B25" s="1">
-        <v>12352</v>
+        <v>12455</v>
       </c>
       <c r="C25" s="1">
-        <v>5288</v>
+        <v>5310</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -11026,8 +9908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11097,10 +9979,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11132,7 +10014,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>4014.07</v>
@@ -11147,7 +10029,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>921</v>
@@ -11162,7 +10044,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>583.97</v>
@@ -11177,7 +10059,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>343.6</v>
@@ -11192,7 +10074,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>115.69999999999899</v>
@@ -11207,7 +10089,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>68.5</v>
@@ -11222,7 +10104,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>35</v>
@@ -11237,7 +10119,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>17.05</v>
@@ -11252,7 +10134,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="B11">
         <v>41.559999999999903</v>
@@ -11267,7 +10149,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>58</v>
@@ -11282,7 +10164,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>13.6</v>
@@ -11297,7 +10179,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -11312,7 +10194,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -11327,7 +10209,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>6.6</v>
@@ -11342,7 +10224,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -11357,7 +10239,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -11372,7 +10254,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -11387,7 +10269,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -11404,6 +10286,215 @@
       <c r="C21">
         <f>SUM(C3:C20)</f>
         <v>11371065.269999988</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>4014.07</v>
+      </c>
+      <c r="C26">
+        <v>7120196.6099999901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>921</v>
+      </c>
+      <c r="C27">
+        <v>1793471.87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>583.97</v>
+      </c>
+      <c r="C28">
+        <v>1057991.42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>343.6</v>
+      </c>
+      <c r="C29">
+        <v>596408.72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>115.69999999999899</v>
+      </c>
+      <c r="C30">
+        <v>259459.20000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>68.5</v>
+      </c>
+      <c r="C31">
+        <v>131637.93999999901</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>58</v>
+      </c>
+      <c r="C32">
+        <v>65078.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>41.559999999999903</v>
+      </c>
+      <c r="C33">
+        <v>66513.459999999905</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>87538.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>17.05</v>
+      </c>
+      <c r="C35">
+        <v>86013.05</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>13.6</v>
+      </c>
+      <c r="C36">
+        <v>24600</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>18675</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>6118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>6.6</v>
+      </c>
+      <c r="C39">
+        <v>17689</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>13059</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>4966</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>18551</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>3098</v>
       </c>
     </row>
   </sheetData>
@@ -11419,11 +10510,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11443,883 +10533,594 @@
         <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1">
-        <v>401235</v>
+        <v>11462.370000000101</v>
       </c>
       <c r="C2" s="1">
-        <v>1146644104.78578</v>
+        <v>19819608.52</v>
+      </c>
+      <c r="D2" s="19">
+        <f>C2/$C$11</f>
+        <v>0.73197762927884924</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C3" s="17"/>
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2756.2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5514751.9699999997</v>
+      </c>
+      <c r="D3" s="19">
+        <f t="shared" ref="D3:D10" si="0">C3/$C$11</f>
+        <v>0.20367077730057323</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1">
-        <v>30884</v>
+        <v>462</v>
       </c>
       <c r="C4" s="1">
-        <v>109913150.92889901</v>
+        <v>1116075.45</v>
       </c>
       <c r="D4" s="19">
-        <f>C4/$C$13</f>
-        <v>0.45994905902403643</v>
+        <f t="shared" si="0"/>
+        <v>4.1218889927263046E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1">
-        <v>11690</v>
+        <v>36.01</v>
       </c>
       <c r="C5" s="1">
-        <v>59732009.256700002</v>
+        <v>170758.81</v>
       </c>
       <c r="D5" s="19">
-        <f t="shared" ref="D5:D11" si="0">C5/$C$13</f>
-        <v>0.24995809163005861</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>6.306463056328696E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1">
-        <v>24159</v>
+        <v>69.8</v>
       </c>
       <c r="C6" s="1">
-        <v>33541543.512099899</v>
+        <v>123450.07</v>
       </c>
       <c r="D6" s="19">
         <f t="shared" si="0"/>
-        <v>0.14035992277742862</v>
+        <v>4.5592570348563068E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1">
-        <v>12452</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1">
-        <v>25342259.097399998</v>
+        <v>161118.82</v>
       </c>
       <c r="D7" s="19">
         <f t="shared" si="0"/>
-        <v>0.10604871325117979</v>
+        <v>5.9504390198624191E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1">
-        <v>3565</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>6220292.0726999799</v>
+        <v>89890</v>
       </c>
       <c r="D8" s="19">
         <f t="shared" si="0"/>
-        <v>2.6029801361474696E-2</v>
+        <v>3.3198167879794106E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1">
-        <v>2005</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1">
-        <v>4016471.4613999999</v>
+        <v>44407.31</v>
       </c>
       <c r="D9" s="19">
         <f t="shared" si="0"/>
-        <v>1.6807563550451401E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>1.6400504310491262E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>44.49</v>
       </c>
       <c r="C10" s="1">
-        <v>2195</v>
+        <v>36734.47</v>
       </c>
       <c r="D10" s="19">
         <f t="shared" si="0"/>
-        <v>9.1853265603389518E-6</v>
+        <v>1.356677163238692E-3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C11" s="17">
+        <f>SUM(C2:C10)</f>
+        <v>27076795.419999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4843.6699999999701</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8723268.0099999998</v>
+      </c>
+      <c r="D15" s="15">
+        <f>C15/$C$24</f>
+        <v>0.33048745149096787</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2698.1099999999901</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4812175.92</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" ref="D16:D23" si="1">C16/$C$24</f>
+        <v>0.18231283896171427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2640.3799999999901</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4999892.5999999903</v>
+      </c>
+      <c r="D17" s="15">
+        <f t="shared" si="1"/>
+        <v>0.18942462402946919</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="1">
-        <v>46</v>
-      </c>
-      <c r="C11" s="1">
-        <v>200174.75109999999</v>
-      </c>
-      <c r="D11" s="19">
-        <f t="shared" si="0"/>
-        <v>8.3766307881005407E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="17">
-        <f>SUM(C4:C11)</f>
-        <v>238968096.0802989</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18">
-        <v>4804</v>
-      </c>
-      <c r="D18">
-        <v>51117983.771899998</v>
-      </c>
-      <c r="E18" s="18">
-        <f>D18/$D$23</f>
-        <v>0.4650900892377488</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>1803.65</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3040707.08</v>
+      </c>
+      <c r="D18" s="15">
+        <f t="shared" si="1"/>
+        <v>0.11519943356638225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19">
-        <v>16127</v>
-      </c>
-      <c r="D19">
-        <v>34985664.7227</v>
-      </c>
-      <c r="E19" s="18">
-        <f t="shared" ref="E19:E23" si="1">D19/$D$23</f>
-        <v>0.31831235755560222</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1088.4000000000001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1998863.04</v>
+      </c>
+      <c r="D19" s="15">
+        <f t="shared" si="1"/>
+        <v>7.5728402613768661E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20">
-        <v>9595</v>
-      </c>
-      <c r="D20">
-        <v>21448416.335299902</v>
-      </c>
-      <c r="E20" s="18">
+        <v>57</v>
+      </c>
+      <c r="B20" s="1">
+        <v>884.31000000000097</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1411684</v>
+      </c>
+      <c r="D20" s="15">
         <f t="shared" si="1"/>
-        <v>0.1951455267075031</v>
+        <v>5.3482690997886176E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21">
-        <v>196</v>
-      </c>
-      <c r="D21">
-        <v>1882290.1839999999</v>
-      </c>
-      <c r="E21" s="18">
+        <v>58</v>
+      </c>
+      <c r="B21" s="1">
+        <v>299</v>
+      </c>
+      <c r="C21" s="1">
+        <v>738766.34999999905</v>
+      </c>
+      <c r="D21" s="15">
         <f t="shared" si="1"/>
-        <v>1.71257636755449E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.7988708816340042E-2</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22">
-        <v>161</v>
-      </c>
-      <c r="D22">
-        <v>475498.91499999998</v>
-      </c>
-      <c r="E22" s="18">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1">
+        <v>169.94999999999899</v>
+      </c>
+      <c r="C22" s="1">
+        <v>292490.41999999899</v>
+      </c>
+      <c r="D22" s="15">
         <f t="shared" si="1"/>
-        <v>4.3262628236008542E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D23">
-        <f>SUM(D18:D22)</f>
-        <v>109909853.92889991</v>
-      </c>
-      <c r="E23" s="18">
+        <v>1.1081215592655222E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="1">
+        <v>163</v>
+      </c>
+      <c r="C23" s="1">
+        <v>377309.1</v>
+      </c>
+      <c r="D23" s="15">
         <f t="shared" si="1"/>
+        <v>1.429463393081634E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <f>SUM(C15:C23)</f>
+        <v>26395156.519999988</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3561.51999999998</v>
+      </c>
+      <c r="D27" s="1">
+        <v>6023538.4499999899</v>
+      </c>
+      <c r="E27" s="18">
+        <f>D27/$D$33</f>
+        <v>0.31768745851857477</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2536.70999999999</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4480761.29</v>
+      </c>
+      <c r="E28" s="18">
+        <f t="shared" ref="E28:E33" si="2">D28/$D$33</f>
+        <v>0.23631984393633496</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1911.27999999999</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3677571.02</v>
+      </c>
+      <c r="E29" s="18">
+        <f t="shared" si="2"/>
+        <v>0.19395878362250094</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1426.1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2319922.6099999901</v>
+      </c>
+      <c r="E30" s="18">
+        <f t="shared" si="2"/>
+        <v>0.12235504497039888</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="1">
+        <v>867.56</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1382305.92</v>
+      </c>
+      <c r="E31" s="18">
+        <f t="shared" si="2"/>
+        <v>7.2904200457121843E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="1">
+        <v>652.65</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1076480.6399999999</v>
+      </c>
+      <c r="E32" s="18">
+        <f t="shared" si="2"/>
+        <v>5.6774668495068598E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D33" s="17">
+        <f>SUM(D27:D32)</f>
+        <v>18960579.929999981</v>
+      </c>
+      <c r="E33" s="18">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="1">
-        <v>401235</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1146644104.78578</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="1">
-        <v>4804</v>
-      </c>
-      <c r="D32" s="1">
-        <v>51117983.771899998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="1">
-        <v>9954</v>
-      </c>
-      <c r="D33" s="1">
-        <v>9424634.7225999907</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="1">
-        <v>16127</v>
-      </c>
-      <c r="D34" s="1">
-        <v>34985664.7227</v>
-      </c>
+    <row r="34" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1">
-        <v>7716</v>
-      </c>
-      <c r="D35" s="1">
-        <v>15666022.6312999</v>
-      </c>
-      <c r="E35" s="18">
-        <f>D35/$D$54</f>
-        <v>0.20123209274142945</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="18"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C36" s="1">
-        <v>6790</v>
+        <v>1280.1500000000001</v>
       </c>
       <c r="D36" s="1">
-        <v>3653085.7158999899</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2693072.5599999898</v>
+      </c>
+      <c r="E36" s="18">
+        <f>D36/$D$39</f>
+        <v>0.56861718734885203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C37" s="1">
-        <v>9595</v>
+        <v>729.099999999999</v>
       </c>
       <c r="D37" s="1">
-        <v>21448416.335299902</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1322321.58</v>
+      </c>
+      <c r="E37" s="18">
+        <f t="shared" ref="E37:E38" si="3">D37/$D$39</f>
+        <v>0.27919588530889522</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C38" s="1">
-        <v>196</v>
+        <v>377.54999999999899</v>
       </c>
       <c r="D38" s="1">
-        <v>1882290.1839999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="1">
-        <v>161</v>
-      </c>
+        <v>720784.47</v>
+      </c>
+      <c r="E38" s="18">
+        <f t="shared" si="3"/>
+        <v>0.15218692734225273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="1"/>
       <c r="D39" s="1">
-        <v>475498.91499999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="1">
-        <v>2543</v>
-      </c>
-      <c r="D40" s="1">
-        <v>4586657.0727000004</v>
-      </c>
-      <c r="E40" s="18">
-        <f>D40/$D$54</f>
-        <v>5.8916205034877739E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="1">
-        <v>2357</v>
-      </c>
-      <c r="D41" s="1">
-        <v>10666213.4197999</v>
-      </c>
+        <f>SUM(D36:D38)</f>
+        <v>4736178.6099999901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1341</v>
-      </c>
-      <c r="D42" s="1">
-        <v>2183816.7108999901</v>
-      </c>
-      <c r="E42" s="18">
-        <f>D42/$D$54</f>
-        <v>2.8051408914736529E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1945</v>
-      </c>
-      <c r="D43" s="1">
-        <v>685554.3321</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1919</v>
-      </c>
-      <c r="D44" s="1">
-        <v>3318147.71559999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1">
-        <v>3297</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="1">
-        <v>431</v>
-      </c>
-      <c r="D46" s="1">
-        <v>2387942.1647000001</v>
-      </c>
-      <c r="E46" s="18">
-        <f>D46/$D$54</f>
-        <v>3.0673426845943975E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1232</v>
-      </c>
-      <c r="D47" s="1">
-        <v>4006763.8974000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" s="1">
-        <v>997</v>
-      </c>
-      <c r="D48" s="1">
-        <v>2178119.4386999998</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" s="1">
-        <v>836</v>
-      </c>
-      <c r="D49" s="1">
-        <v>3210884.9550999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="1">
-        <v>502</v>
-      </c>
-      <c r="D50" s="1">
-        <v>470990.63679999899</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="1">
-        <v>439</v>
-      </c>
-      <c r="D51" s="1">
-        <v>687302.498599999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" s="1">
-        <v>315</v>
-      </c>
-      <c r="D52" s="1">
-        <v>339514.2427</v>
-      </c>
-      <c r="E52" s="18">
-        <f>D52/$D$54</f>
-        <v>4.3611044859299805E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>48</v>
-      </c>
-      <c r="C53" s="1">
-        <v>376</v>
-      </c>
-      <c r="D53" s="1">
-        <v>337305.61909999902</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="3:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="3:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="3:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="3:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="3:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="3:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C54" s="1"/>
-      <c r="D54" s="1">
-        <f>SUM(D35:D52)</f>
-        <v>77850517.866599694</v>
-      </c>
-      <c r="E54">
-        <f>D54/$D$54</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" s="1">
-        <v>34</v>
-      </c>
-      <c r="D55" s="1">
-        <v>161632.20879999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" t="s">
-        <v>46</v>
-      </c>
-      <c r="C56" s="1">
-        <v>165</v>
-      </c>
-      <c r="D56" s="1">
-        <v>717603.49949999899</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>39</v>
-      </c>
-      <c r="C57" s="1">
-        <v>12</v>
-      </c>
-      <c r="D57" s="1">
-        <v>38542.542300000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="1">
-        <v>128</v>
-      </c>
-      <c r="D58" s="1">
-        <v>195415.40759999899</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>51</v>
-      </c>
-      <c r="B61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="1">
-        <v>34</v>
-      </c>
-      <c r="D61" s="1">
-        <v>115768.1529</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>53</v>
-      </c>
-      <c r="B62" t="s">
-        <v>35</v>
-      </c>
-      <c r="C62" s="1">
-        <v>5005</v>
-      </c>
-      <c r="D62" s="1">
-        <v>46028724.406199902</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" t="s">
-        <v>39</v>
-      </c>
-      <c r="C63" s="1">
-        <v>1967</v>
-      </c>
-      <c r="D63" s="1">
-        <v>3967875.1956000002</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64" t="s">
-        <v>49</v>
-      </c>
-      <c r="C64" s="1">
-        <v>22</v>
-      </c>
-      <c r="D64" s="1">
-        <v>7313.88309999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B65" t="s">
-        <v>36</v>
-      </c>
-      <c r="C65" s="1">
-        <v>16</v>
-      </c>
-      <c r="D65" s="1">
-        <v>52497.326999999997</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" s="1">
-        <v>5002</v>
-      </c>
-      <c r="D66" s="1">
-        <v>10734780.008899899</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>51</v>
-      </c>
-      <c r="B67" t="s">
-        <v>62</v>
-      </c>
-      <c r="C67" s="1">
-        <v>9</v>
-      </c>
-      <c r="D67" s="1">
-        <v>29112.815999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>55</v>
-      </c>
-      <c r="B68" t="s">
-        <v>30</v>
-      </c>
-      <c r="C68" s="1">
-        <v>38</v>
-      </c>
-      <c r="D68" s="1">
-        <v>48596.265800000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>54</v>
-      </c>
-      <c r="B69" t="s">
-        <v>63</v>
-      </c>
-      <c r="C69" s="1">
-        <v>1</v>
-      </c>
-      <c r="D69" s="1">
-        <v>2272.547</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>57</v>
-      </c>
-      <c r="B70" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="1">
-        <v>2195</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>54</v>
-      </c>
-      <c r="B71" t="s">
-        <v>64</v>
-      </c>
-      <c r="C71" s="1">
-        <v>1</v>
-      </c>
-      <c r="D71" s="1">
-        <v>1749.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>53</v>
-      </c>
-      <c r="B72" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72" s="1">
-        <v>1683</v>
-      </c>
-      <c r="D72" s="1">
-        <v>2968504.8415999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>54</v>
-      </c>
-      <c r="B73" t="s">
-        <v>41</v>
-      </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="1">
-        <v>1099.5</v>
-      </c>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="3:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="3:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A30:D73">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="CASUALE"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A35:D38">
+    <sortState ref="A45:D47">
+      <sortCondition descending="1" ref="D44:D47"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>